<commit_message>
links changed to local
</commit_message>
<xml_diff>
--- a/calendar_school_unique.xlsx
+++ b/calendar_school_unique.xlsx
@@ -35,50 +35,50 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="004C0F89"/>
+        <bgColor rgb="004C0F89"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00F4E0A3"/>
+        <bgColor rgb="00F4E0A3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00633535"/>
+        <bgColor rgb="00633535"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004C890F"/>
+        <bgColor rgb="004C890F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00A3B7F4"/>
+        <bgColor rgb="00A3B7F4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00DBBCD3"/>
+        <bgColor rgb="00DBBCD3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="00BCDBC4"/>
         <bgColor rgb="00BCDBC4"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00F4E0A3"/>
-        <bgColor rgb="00F4E0A3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="00356363"/>
         <bgColor rgb="00356363"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00A3B7F4"/>
-        <bgColor rgb="00A3B7F4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="004C890F"/>
-        <bgColor rgb="004C890F"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00633535"/>
-        <bgColor rgb="00633535"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00DBBCD3"/>
-        <bgColor rgb="00DBBCD3"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="004C0F89"/>
-        <bgColor rgb="004C0F89"/>
       </patternFill>
     </fill>
   </fills>
@@ -100,10 +100,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -469,7 +469,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AT5"/>
+  <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -499,229 +499,111 @@
     <col width="3" customWidth="1" min="20" max="20"/>
     <col width="3" customWidth="1" min="21" max="21"/>
     <col width="3" customWidth="1" min="22" max="22"/>
-    <col width="3" customWidth="1" min="23" max="23"/>
-    <col width="3" customWidth="1" min="24" max="24"/>
-    <col width="3" customWidth="1" min="25" max="25"/>
-    <col width="3" customWidth="1" min="26" max="26"/>
-    <col width="3" customWidth="1" min="27" max="27"/>
-    <col width="3" customWidth="1" min="28" max="28"/>
-    <col width="3" customWidth="1" min="29" max="29"/>
-    <col width="3" customWidth="1" min="30" max="30"/>
-    <col width="3" customWidth="1" min="31" max="31"/>
-    <col width="3" customWidth="1" min="32" max="32"/>
-    <col width="3" customWidth="1" min="33" max="33"/>
-    <col width="3" customWidth="1" min="34" max="34"/>
-    <col width="3" customWidth="1" min="35" max="35"/>
-    <col width="3" customWidth="1" min="36" max="36"/>
-    <col width="3" customWidth="1" min="37" max="37"/>
-    <col width="3" customWidth="1" min="38" max="38"/>
-    <col width="3" customWidth="1" min="39" max="39"/>
-    <col width="3" customWidth="1" min="40" max="40"/>
-    <col width="3" customWidth="1" min="41" max="41"/>
-    <col width="3" customWidth="1" min="42" max="42"/>
-    <col width="3" customWidth="1" min="43" max="43"/>
-    <col width="3" customWidth="1" min="44" max="44"/>
-    <col width="3" customWidth="1" min="45" max="45"/>
-    <col width="3" customWidth="1" min="46" max="46"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="n"/>
-      <c r="B1" s="1" t="n"/>
+      <c r="B1" s="2" t="n"/>
       <c r="C1" s="2" t="n"/>
-      <c r="E1" s="2" t="n"/>
+      <c r="E1" s="3" t="n"/>
       <c r="F1" s="3" t="n"/>
       <c r="G1" s="4" t="n"/>
       <c r="H1" s="4" t="n"/>
       <c r="I1" s="4" t="n"/>
-      <c r="M1" s="5" t="n"/>
-      <c r="N1" s="5" t="n"/>
-      <c r="O1" s="5" t="n"/>
-      <c r="Q1" s="1" t="n"/>
-      <c r="R1" s="6" t="n"/>
+      <c r="J1" s="5" t="n"/>
+      <c r="M1" s="6" t="n"/>
+      <c r="N1" s="2" t="n"/>
+      <c r="O1" s="2" t="n"/>
+      <c r="Q1" s="7" t="n"/>
+      <c r="R1" s="7" t="n"/>
       <c r="S1" s="7" t="n"/>
-      <c r="T1" s="7" t="n"/>
-      <c r="U1" s="4" t="n"/>
-      <c r="Y1" s="8" t="n"/>
-      <c r="Z1" s="8" t="n"/>
-      <c r="AA1" s="7" t="n"/>
-      <c r="AC1" s="7" t="n"/>
-      <c r="AD1" s="6" t="n"/>
-      <c r="AE1" s="5" t="n"/>
-      <c r="AF1" s="5" t="n"/>
-      <c r="AG1" s="5" t="n"/>
-      <c r="AK1" s="1" t="n"/>
-      <c r="AL1" s="4" t="n"/>
-      <c r="AM1" s="4" t="n"/>
-      <c r="AO1" s="4" t="n"/>
-      <c r="AP1" s="2" t="n"/>
-      <c r="AQ1" s="2" t="n"/>
-      <c r="AR1" s="2" t="n"/>
-      <c r="AS1" s="2" t="n"/>
+      <c r="T1" s="3" t="n"/>
+      <c r="U1" s="8" t="n"/>
+      <c r="V1" s="8" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n"/>
-      <c r="B2" s="2" t="n"/>
+      <c r="B2" s="1" t="n"/>
       <c r="C2" s="2" t="n"/>
-      <c r="D2" s="2" t="n"/>
-      <c r="E2" s="2" t="n"/>
+      <c r="D2" s="7" t="n"/>
+      <c r="E2" s="3" t="n"/>
       <c r="F2" s="3" t="n"/>
-      <c r="G2" s="4" t="n"/>
-      <c r="H2" s="7" t="n"/>
-      <c r="I2" s="4" t="n"/>
-      <c r="J2" s="4" t="n"/>
-      <c r="M2" s="5" t="n"/>
-      <c r="N2" s="5" t="n"/>
-      <c r="O2" s="2" t="n"/>
-      <c r="P2" s="2" t="n"/>
-      <c r="Q2" s="1" t="n"/>
-      <c r="R2" s="6" t="n"/>
-      <c r="S2" s="6" t="n"/>
-      <c r="T2" s="7" t="n"/>
-      <c r="U2" s="4" t="n"/>
-      <c r="V2" s="4" t="n"/>
-      <c r="Y2" s="8" t="n"/>
-      <c r="Z2" s="8" t="n"/>
-      <c r="AA2" s="7" t="n"/>
-      <c r="AB2" s="7" t="n"/>
-      <c r="AC2" s="7" t="n"/>
-      <c r="AD2" s="6" t="n"/>
-      <c r="AE2" s="4" t="n"/>
-      <c r="AF2" s="5" t="n"/>
-      <c r="AG2" s="5" t="n"/>
-      <c r="AH2" s="3" t="n"/>
-      <c r="AK2" s="1" t="n"/>
-      <c r="AL2" s="5" t="n"/>
-      <c r="AM2" s="4" t="n"/>
-      <c r="AN2" s="4" t="n"/>
-      <c r="AO2" s="4" t="n"/>
-      <c r="AP2" s="2" t="n"/>
-      <c r="AQ2" s="7" t="n"/>
-      <c r="AR2" s="2" t="n"/>
-      <c r="AS2" s="3" t="n"/>
-      <c r="AT2" s="3" t="n"/>
+      <c r="G2" s="3" t="n"/>
+      <c r="H2" s="4" t="n"/>
+      <c r="I2" s="5" t="n"/>
+      <c r="J2" s="5" t="n"/>
+      <c r="M2" s="6" t="n"/>
+      <c r="N2" s="2" t="n"/>
+      <c r="O2" s="4" t="n"/>
+      <c r="P2" s="4" t="n"/>
+      <c r="Q2" s="7" t="n"/>
+      <c r="R2" s="7" t="n"/>
+      <c r="S2" s="3" t="n"/>
+      <c r="T2" s="3" t="n"/>
+      <c r="U2" s="8" t="n"/>
+      <c r="V2" s="8" t="n"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n"/>
-      <c r="B3" s="8" t="n"/>
-      <c r="C3" s="8" t="n"/>
-      <c r="E3" s="5" t="n"/>
-      <c r="F3" s="3" t="n"/>
-      <c r="G3" s="3" t="n"/>
-      <c r="H3" s="7" t="n"/>
-      <c r="I3" s="7" t="n"/>
-      <c r="J3" s="7" t="n"/>
-      <c r="M3" s="5" t="n"/>
-      <c r="N3" s="8" t="n"/>
+      <c r="B3" s="2" t="n"/>
+      <c r="C3" s="2" t="n"/>
+      <c r="D3" s="7" t="n"/>
+      <c r="E3" s="7" t="n"/>
+      <c r="G3" s="4" t="n"/>
+      <c r="H3" s="4" t="n"/>
+      <c r="I3" s="5" t="n"/>
+      <c r="M3" s="6" t="n"/>
+      <c r="N3" s="2" t="n"/>
       <c r="O3" s="2" t="n"/>
-      <c r="Q3" s="1" t="n"/>
-      <c r="R3" s="6" t="n"/>
-      <c r="S3" s="7" t="n"/>
-      <c r="T3" s="7" t="n"/>
-      <c r="U3" s="7" t="n"/>
-      <c r="V3" s="4" t="n"/>
-      <c r="Y3" s="2" t="n"/>
-      <c r="Z3" s="8" t="n"/>
-      <c r="AA3" s="2" t="n"/>
-      <c r="AC3" s="7" t="n"/>
-      <c r="AD3" s="6" t="n"/>
-      <c r="AE3" s="4" t="n"/>
-      <c r="AF3" s="4" t="n"/>
-      <c r="AG3" s="5" t="n"/>
-      <c r="AH3" s="3" t="n"/>
-      <c r="AK3" s="1" t="n"/>
-      <c r="AL3" s="5" t="n"/>
-      <c r="AM3" s="5" t="n"/>
-      <c r="AO3" s="7" t="n"/>
-      <c r="AP3" s="7" t="n"/>
-      <c r="AQ3" s="7" t="n"/>
-      <c r="AR3" s="8" t="n"/>
-      <c r="AS3" s="3" t="n"/>
-      <c r="AT3" s="3" t="n"/>
+      <c r="P3" s="4" t="n"/>
+      <c r="Q3" s="7" t="n"/>
+      <c r="S3" s="3" t="n"/>
+      <c r="T3" s="3" t="n"/>
+      <c r="U3" s="8" t="n"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n"/>
-      <c r="B4" s="8" t="n"/>
-      <c r="C4" s="8" t="n"/>
-      <c r="D4" s="5" t="n"/>
-      <c r="E4" s="5" t="n"/>
-      <c r="F4" s="3" t="n"/>
-      <c r="G4" s="3" t="n"/>
-      <c r="H4" s="7" t="n"/>
-      <c r="I4" s="6" t="n"/>
-      <c r="J4" s="7" t="n"/>
-      <c r="M4" s="8" t="n"/>
-      <c r="N4" s="8" t="n"/>
-      <c r="O4" s="2" t="n"/>
-      <c r="P4" s="2" t="n"/>
-      <c r="Q4" s="1" t="n"/>
-      <c r="R4" s="6" t="n"/>
-      <c r="S4" s="3" t="n"/>
-      <c r="T4" s="3" t="n"/>
-      <c r="U4" s="4" t="n"/>
-      <c r="V4" s="4" t="n"/>
-      <c r="Y4" s="2" t="n"/>
-      <c r="Z4" s="2" t="n"/>
-      <c r="AA4" s="2" t="n"/>
-      <c r="AB4" s="2" t="n"/>
-      <c r="AC4" s="1" t="n"/>
-      <c r="AD4" s="6" t="n"/>
-      <c r="AE4" s="6" t="n"/>
-      <c r="AF4" s="4" t="n"/>
-      <c r="AG4" s="3" t="n"/>
-      <c r="AH4" s="3" t="n"/>
-      <c r="AK4" s="1" t="n"/>
-      <c r="AL4" s="5" t="n"/>
-      <c r="AM4" s="5" t="n"/>
-      <c r="AN4" s="5" t="n"/>
-      <c r="AO4" s="7" t="n"/>
-      <c r="AP4" s="6" t="n"/>
-      <c r="AQ4" s="7" t="n"/>
-      <c r="AR4" s="8" t="n"/>
-      <c r="AS4" s="8" t="n"/>
-      <c r="AT4" s="3" t="n"/>
+      <c r="B4" s="6" t="n"/>
+      <c r="C4" s="2" t="n"/>
+      <c r="D4" s="7" t="n"/>
+      <c r="E4" s="7" t="n"/>
+      <c r="F4" s="7" t="n"/>
+      <c r="G4" s="8" t="n"/>
+      <c r="H4" s="8" t="n"/>
+      <c r="I4" s="5" t="n"/>
+      <c r="J4" s="5" t="n"/>
+      <c r="M4" s="6" t="n"/>
+      <c r="N4" s="2" t="n"/>
+      <c r="O4" s="4" t="n"/>
+      <c r="P4" s="4" t="n"/>
+      <c r="Q4" s="4" t="n"/>
+      <c r="R4" s="1" t="n"/>
+      <c r="S4" s="5" t="n"/>
+      <c r="T4" s="5" t="n"/>
+      <c r="U4" s="8" t="n"/>
+      <c r="V4" s="5" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n"/>
-      <c r="B5" s="8" t="n"/>
-      <c r="C5" s="5" t="n"/>
-      <c r="D5" s="5" t="n"/>
-      <c r="E5" s="5" t="n"/>
+      <c r="B5" s="6" t="n"/>
+      <c r="C5" s="6" t="n"/>
+      <c r="D5" s="6" t="n"/>
+      <c r="E5" s="6" t="n"/>
       <c r="F5" s="6" t="n"/>
-      <c r="G5" s="6" t="n"/>
-      <c r="H5" s="6" t="n"/>
-      <c r="I5" s="6" t="n"/>
-      <c r="J5" s="6" t="n"/>
-      <c r="M5" s="8" t="n"/>
-      <c r="N5" s="8" t="n"/>
-      <c r="O5" s="2" t="n"/>
+      <c r="G5" s="8" t="n"/>
+      <c r="H5" s="8" t="n"/>
+      <c r="I5" s="8" t="n"/>
+      <c r="J5" s="8" t="n"/>
+      <c r="M5" s="6" t="n"/>
+      <c r="N5" s="6" t="n"/>
+      <c r="O5" s="1" t="n"/>
       <c r="P5" s="1" t="n"/>
       <c r="Q5" s="1" t="n"/>
-      <c r="R5" s="6" t="n"/>
-      <c r="S5" s="3" t="n"/>
-      <c r="T5" s="3" t="n"/>
-      <c r="U5" s="3" t="n"/>
-      <c r="V5" s="3" t="n"/>
-      <c r="Y5" s="1" t="n"/>
-      <c r="Z5" s="1" t="n"/>
-      <c r="AA5" s="1" t="n"/>
-      <c r="AB5" s="1" t="n"/>
-      <c r="AC5" s="1" t="n"/>
-      <c r="AD5" s="6" t="n"/>
-      <c r="AE5" s="4" t="n"/>
-      <c r="AF5" s="4" t="n"/>
-      <c r="AG5" s="3" t="n"/>
-      <c r="AH5" s="3" t="n"/>
-      <c r="AK5" s="1" t="n"/>
-      <c r="AL5" s="1" t="n"/>
-      <c r="AM5" s="6" t="n"/>
-      <c r="AN5" s="6" t="n"/>
-      <c r="AO5" s="6" t="n"/>
-      <c r="AP5" s="6" t="n"/>
-      <c r="AQ5" s="6" t="n"/>
-      <c r="AR5" s="8" t="n"/>
-      <c r="AS5" s="8" t="n"/>
-      <c r="AT5" s="3" t="n"/>
+      <c r="R5" s="1" t="n"/>
+      <c r="S5" s="1" t="n"/>
+      <c r="T5" s="5" t="n"/>
+      <c r="U5" s="5" t="n"/>
+      <c r="V5" s="5" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>